<commit_message>
feat: create GT done
</commit_message>
<xml_diff>
--- a/src/files/archivo_actualizado_geOperarioGeneral.xlsx
+++ b/src/files/archivo_actualizado_geOperarioGeneral.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t xml:space="preserve">GUÍA DE ENTRENAMIENTO </t>
   </si>
@@ -42,16 +42,16 @@
     <t xml:space="preserve"> ÁREA</t>
   </si>
   <si>
-    <t>AGUILAR CAMACHO YURITZY AMEYALIN</t>
-  </si>
-  <si>
-    <t>2025-12-22</t>
+    <t>ADALBERTO JOSE MOYA NARVAEZ</t>
+  </si>
+  <si>
+    <t>2026-01-27</t>
   </si>
   <si>
     <t>Operario General</t>
   </si>
   <si>
-    <t>Producción</t>
+    <t>PRODUCCION</t>
   </si>
   <si>
     <t>TEMA</t>
@@ -75,103 +75,46 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>Proceso Fabricación del jabón líquido/Solido/Hidroalcoholico Interactivo</t>
-  </si>
-  <si>
-    <t>LOAIZA FRANCO DIEGO FERNANDO</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>z1</t>
-  </si>
-  <si>
-    <t>Aspectos Seguridad Ocupacional: Levantamiento y movilización de cargas, Seguridad en la Exposición a Material Particulado, Seguridad en la Manipulación de Sustancias Químicas, Manejo de Equipos y Herramientas, Ruido, Almacenamiento y Bodegaje, Proyección de Partículas, Ergonomía Aplicada al Puesto de Trabajo</t>
-  </si>
-  <si>
-    <t>ARRIETA MOSQUEDA OMAR ALFONSO</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Generalidades de Control de Calidad</t>
-  </si>
-  <si>
-    <t>RAMIREZ LOPEZ RAMON</t>
+    <t>Limpieza y Sanitización</t>
+  </si>
+  <si>
+    <t>TORRES RODRIGUEZ DANIELA</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>27 =&gt; 1</t>
+  </si>
+  <si>
+    <t>Defectología</t>
+  </si>
+  <si>
+    <t>2026-01-26</t>
+  </si>
+  <si>
+    <t>PEREA MARCOS JOYCELYNN ANGIE</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>26 =&gt; 2</t>
+  </si>
+  <si>
+    <t>Buenas Practicas de Documentación</t>
+  </si>
+  <si>
+    <t>2026-01-25</t>
+  </si>
+  <si>
+    <t>MELENDEZ CRISTOBAL GONZALO</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Generalidades de Microbiología</t>
-  </si>
-  <si>
-    <t>Generalidades de Buenas Prácticas de Manufactura</t>
-  </si>
-  <si>
-    <t>SALGADO GONZALEZ MARTHA GABRIELA</t>
-  </si>
-  <si>
-    <t>Defectología</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Manejo seguro de sustancias químicas (Operación y Manejo de Sustancias Quimicas)</t>
-  </si>
-  <si>
-    <t>Uso y Manejo de Patrin Hidraulico</t>
-  </si>
-  <si>
-    <t>Reprobado</t>
-  </si>
-  <si>
-    <t>Sistema Integrado de Gestión</t>
-  </si>
-  <si>
-    <t>Manejo de Residuos</t>
-  </si>
-  <si>
-    <t>Manejo de Derrames</t>
-  </si>
-  <si>
-    <t>Limpieza y Sanitización</t>
-  </si>
-  <si>
-    <t>ZUPPA FLAÑO ERNESTO</t>
-  </si>
-  <si>
-    <t>Buenas Practicas de Documentación</t>
-  </si>
-  <si>
-    <t>Manejo y disposición de residuos de Jabon</t>
-  </si>
-  <si>
-    <t>LARIOS FRAGOSO KENIA DENISSE</t>
-  </si>
-  <si>
-    <t>Alistamiento de los materiales y operación de empaque bajo los estandares de calidad</t>
-  </si>
-  <si>
-    <t>ZUPPA FLAÑO ERNESTO / RODRIGUEZ HERNANDEZ ALEXIS</t>
-  </si>
-  <si>
-    <t>Aprobado</t>
-  </si>
-  <si>
-    <t>Manejo de Estibas y patron de arrume</t>
-  </si>
-  <si>
-    <t>Manejo de maquina encintadora y funcionalidad para el sellado de cajas</t>
-  </si>
-  <si>
-    <t>Principios y lineamientos para la correcta codificación e inspección de productos</t>
+    <t>25 =&gt; 3</t>
   </si>
   <si>
     <t>1 DE 2</t>
@@ -1029,591 +972,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="952500" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
@@ -1622,7 +980,7 @@
     <xdr:ext cx="1143000" cy="476250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 20">
+        <xdr:cNvPr id="5" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -1661,7 +1019,7 @@
     <xdr:ext cx="1143000" cy="476250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 21">
+        <xdr:cNvPr id="6" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -1700,7 +1058,7 @@
     <xdr:ext cx="1143000" cy="476250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 22">
+        <xdr:cNvPr id="7" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -1739,7 +1097,7 @@
     <xdr:ext cx="1190625" cy="704850"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="Picture 23">
+        <xdr:cNvPr id="8" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
@@ -2238,11 +1596,11 @@
         <v>18</v>
       </c>
       <c r="B6" s="30"/>
-      <c r="C6" s="31">
-        <v>46012.75</v>
+      <c r="C6" s="31" t="s">
+        <v>8</v>
       </c>
       <c r="D6" s="32">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>19</v>
@@ -2261,395 +1619,215 @@
         <v>22</v>
       </c>
       <c r="B7" s="36"/>
-      <c r="C7" s="31">
-        <v>46012.75</v>
+      <c r="C7" s="31" t="s">
+        <v>23</v>
       </c>
       <c r="D7" s="32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G7" s="33"/>
       <c r="H7" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I7" s="34"/>
     </row>
     <row r="8" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="38"/>
-      <c r="C8" s="31">
-        <v>46012.75</v>
+      <c r="C8" s="31" t="s">
+        <v>28</v>
       </c>
       <c r="D8" s="33">
         <v>1</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G8" s="32"/>
       <c r="H8" s="21" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I8" s="34"/>
     </row>
     <row r="9" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
-        <v>29</v>
-      </c>
+      <c r="A9" s="37"/>
       <c r="B9" s="38"/>
-      <c r="C9" s="31">
-        <v>46006.75</v>
-      </c>
-      <c r="D9" s="33">
-        <v>1</v>
-      </c>
-      <c r="E9" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>24</v>
-      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="32"/>
-      <c r="H9" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H9" s="21"/>
       <c r="I9" s="34"/>
     </row>
     <row r="10" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>30</v>
-      </c>
+      <c r="A10" s="37"/>
       <c r="B10" s="38"/>
-      <c r="C10" s="31">
-        <v>46007.75</v>
-      </c>
-      <c r="D10" s="33">
-        <v>1</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>20</v>
-      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="32"/>
-      <c r="H10" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H10" s="21"/>
       <c r="I10" s="34"/>
     </row>
     <row r="11" ht="36" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>32</v>
-      </c>
+      <c r="A11" s="35"/>
       <c r="B11" s="36"/>
-      <c r="C11" s="31">
-        <v>46007.75</v>
-      </c>
-      <c r="D11" s="33">
-        <v>1</v>
-      </c>
-      <c r="E11" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>33</v>
-      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="32"/>
-      <c r="H11" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H11" s="21"/>
       <c r="I11" s="34"/>
     </row>
     <row r="12" ht="61.5" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>34</v>
-      </c>
+      <c r="A12" s="37"/>
       <c r="B12" s="38"/>
-      <c r="C12" s="31">
-        <v>46006.75</v>
-      </c>
-      <c r="D12" s="32">
-        <v>2</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="33"/>
-      <c r="H12" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H12" s="21"/>
       <c r="I12" s="34"/>
     </row>
     <row r="13" ht="48.75" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>35</v>
-      </c>
+      <c r="A13" s="35"/>
       <c r="B13" s="36"/>
-      <c r="C13" s="31">
-        <v>46012.75</v>
-      </c>
-      <c r="D13" s="32">
-        <v>1</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>36</v>
-      </c>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="40"/>
-      <c r="H13" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H13" s="21"/>
       <c r="I13" s="34"/>
     </row>
     <row r="14" ht="48.75" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
-        <v>37</v>
-      </c>
+      <c r="A14" s="35"/>
       <c r="B14" s="36"/>
-      <c r="C14" s="31">
-        <v>46006.75</v>
-      </c>
-      <c r="D14" s="32">
-        <v>1</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>33</v>
-      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="33"/>
       <c r="G14" s="40"/>
-      <c r="H14" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H14" s="21"/>
       <c r="I14" s="34"/>
     </row>
     <row r="15" ht="34.5" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>38</v>
-      </c>
+      <c r="A15" s="35"/>
       <c r="B15" s="36"/>
-      <c r="C15" s="31">
-        <v>45993.75</v>
-      </c>
-      <c r="D15" s="32">
-        <v>2</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="40"/>
-      <c r="H15" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H15" s="21"/>
       <c r="I15" s="34"/>
     </row>
     <row r="16" ht="34.5" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>39</v>
-      </c>
+      <c r="A16" s="35"/>
       <c r="B16" s="36"/>
-      <c r="C16" s="31">
-        <v>46007.75</v>
-      </c>
-      <c r="D16" s="41">
-        <v>1</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>20</v>
-      </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="40"/>
-      <c r="H16" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H16" s="21"/>
       <c r="I16" s="34"/>
     </row>
     <row r="17" ht="49.5" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>40</v>
-      </c>
+      <c r="A17" s="35"/>
       <c r="B17" s="36"/>
-      <c r="C17" s="31">
-        <v>45993.75</v>
-      </c>
-      <c r="D17" s="41">
-        <v>1</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>28</v>
-      </c>
+      <c r="C17" s="31"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="40"/>
-      <c r="H17" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H17" s="21"/>
       <c r="I17" s="34"/>
     </row>
     <row r="18" ht="48" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>42</v>
-      </c>
+      <c r="A18" s="35"/>
       <c r="B18" s="36"/>
-      <c r="C18" s="31">
-        <v>46007.75</v>
-      </c>
-      <c r="D18" s="41">
-        <v>1</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>24</v>
-      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="42"/>
       <c r="G18" s="40"/>
-      <c r="H18" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H18" s="21"/>
       <c r="I18" s="34"/>
     </row>
     <row r="19" ht="50.25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>43</v>
-      </c>
+      <c r="A19" s="35"/>
       <c r="B19" s="36"/>
-      <c r="C19" s="31">
-        <v>45994.75</v>
-      </c>
-      <c r="D19" s="32">
-        <v>1</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>36</v>
-      </c>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="43"/>
-      <c r="H19" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H19" s="21"/>
       <c r="I19" s="34"/>
     </row>
     <row r="20" ht="58.5" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>45</v>
-      </c>
+      <c r="A20" s="35"/>
       <c r="B20" s="36"/>
-      <c r="C20" s="31">
-        <v>46008.75</v>
-      </c>
-      <c r="D20" s="32">
-        <v>2</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>47</v>
-      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="33"/>
       <c r="G20" s="43"/>
-      <c r="H20" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H20" s="21"/>
       <c r="I20" s="34"/>
     </row>
     <row r="21" ht="66.75" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>48</v>
-      </c>
+      <c r="A21" s="35"/>
       <c r="B21" s="36"/>
-      <c r="C21" s="31">
-        <v>45993.75</v>
-      </c>
-      <c r="D21" s="32">
-        <v>2</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="33" t="s">
-        <v>47</v>
-      </c>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="43"/>
-      <c r="H21" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H21" s="21"/>
       <c r="I21" s="34"/>
     </row>
     <row r="22" ht="53.25" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
-        <v>49</v>
-      </c>
+      <c r="A22" s="35"/>
       <c r="B22" s="36"/>
-      <c r="C22" s="31">
-        <v>46008.75</v>
-      </c>
-      <c r="D22" s="32">
-        <v>1</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="33" t="s">
-        <v>47</v>
-      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="33"/>
       <c r="G22" s="43"/>
-      <c r="H22" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H22" s="21"/>
       <c r="I22" s="34"/>
     </row>
     <row r="23" ht="54.75" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>50</v>
-      </c>
+      <c r="A23" s="35"/>
       <c r="B23" s="36"/>
-      <c r="C23" s="31">
-        <v>46007.75</v>
-      </c>
-      <c r="D23" s="32">
-        <v>1</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="33" t="s">
-        <v>36</v>
-      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="43"/>
-      <c r="H23" s="21" t="s">
-        <v>25</v>
-      </c>
+      <c r="H23" s="21"/>
       <c r="I23" s="34"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -2662,14 +1840,14 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B25" s="46"/>
       <c r="C25" s="46"/>
       <c r="D25" s="46"/>
       <c r="E25" s="11"/>
       <c r="F25" s="47">
-        <v>3.33</v>
+        <v>2</v>
       </c>
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
@@ -2677,7 +1855,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="50" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B26" s="51"/>
       <c r="C26" s="51"/>
@@ -2690,7 +1868,7 @@
     </row>
     <row r="27" ht="24.75" customHeight="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B27" s="54"/>
       <c r="C27" s="54"/>
@@ -2741,13 +1919,13 @@
       <c r="B31" s="68"/>
       <c r="C31" s="69"/>
       <c r="D31" s="68" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="E31" s="68"/>
       <c r="F31" s="68"/>
       <c r="G31" s="69"/>
       <c r="H31" s="70" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="I31" s="71"/>
     </row>
@@ -2757,7 +1935,7 @@
       <c r="C32" s="73"/>
       <c r="D32" s="73"/>
       <c r="E32" s="64" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F32" s="73"/>
       <c r="G32" s="73"/>

</xml_diff>